<commit_message>
Update Programming DocPac pt2.xlsx
</commit_message>
<xml_diff>
--- a/Exports/Programming DocPac pt2.xlsx
+++ b/Exports/Programming DocPac pt2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveycstech-my.sharepoint.com/personal/jessi2022619_live_ytech_edu/Documents/Documents/GitHub/docpacs2122/Exports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkipp\OneDrive - York County School of Technology\Documents\GitHub\docpacs2122\Exports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="8_{CAEEA85D-BC51-406A-A0F1-E32D4FDF477E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{7ACB1F28-2A6C-4D4F-BE67-76D6308F91EB}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{CAEEA85D-BC51-406A-A0F1-E32D4FDF477E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{0CE3F3B4-E96C-4652-B6F0-BDB10FC5E230}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="4" xr2:uid="{32484C1D-9C75-4957-8604-D1053A17B984}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="210">
   <si>
     <t>Date</t>
   </si>
@@ -446,6 +446,219 @@
   </si>
   <si>
     <t>Final DocPac Submissions</t>
+  </si>
+  <si>
+    <t>Jan7</t>
+  </si>
+  <si>
+    <t>Examine requirements for the NOCTI</t>
+  </si>
+  <si>
+    <t>Develop a plan to pass the preformance NOCTI</t>
+  </si>
+  <si>
+    <t>Practiced the skills required in our plan</t>
+  </si>
+  <si>
+    <t>Design a Routine</t>
+  </si>
+  <si>
+    <t>Lesson Key Take-Aways x 3</t>
+  </si>
+  <si>
+    <t>JS Challenge Pt. 3</t>
+  </si>
+  <si>
+    <t>Reflection questions have changed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan 3rd                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan 5th         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan 7th          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                         </t>
+  </si>
+  <si>
+    <t>Examining the NOCTI Requirements</t>
+  </si>
+  <si>
+    <t>Building NOCTI Flowchart</t>
+  </si>
+  <si>
+    <t>Programming NOCTI Application</t>
+  </si>
+  <si>
+    <t>Jan14</t>
+  </si>
+  <si>
+    <t>Develop a Daily Routine</t>
+  </si>
+  <si>
+    <t>Design a flow chart for the Exam</t>
+  </si>
+  <si>
+    <t>Practice the skills required to pass the Exam</t>
+  </si>
+  <si>
+    <t>Present Team Projects to Teacher</t>
+  </si>
+  <si>
+    <t>Team Project Presentation</t>
+  </si>
+  <si>
+    <t>Lesson Key Take-Aways x 2</t>
+  </si>
+  <si>
+    <t>JS Challenge Pt. 4</t>
+  </si>
+  <si>
+    <t>JS Challenge Pt. 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exam Preparation Progress Report </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan 10th      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan 11th         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan 13th      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan 14th         </t>
+  </si>
+  <si>
+    <t>DocPac Jan07 Due</t>
+  </si>
+  <si>
+    <t>Routines</t>
+  </si>
+  <si>
+    <t>nodeJS Debugging with Chrome</t>
+  </si>
+  <si>
+    <t>Building Exam Flowchart</t>
+  </si>
+  <si>
+    <t>Team Project Presentations</t>
+  </si>
+  <si>
+    <t>Jan21</t>
+  </si>
+  <si>
+    <t>Prepare for Exam</t>
+  </si>
+  <si>
+    <t>Pass Exam</t>
+  </si>
+  <si>
+    <t>Exam Preparation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan 18th      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan 19th       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan 20th      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan 21st        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                        </t>
+  </si>
+  <si>
+    <t>Exam Prep</t>
+  </si>
+  <si>
+    <t>Exam</t>
+  </si>
+  <si>
+    <t>Jan28</t>
+  </si>
+  <si>
+    <t>Review reading/Writing to JSON foles for Exam</t>
+  </si>
+  <si>
+    <t>Prepare DocPac Binders for grading and review</t>
+  </si>
+  <si>
+    <t>DocPac Binder Audit</t>
+  </si>
+  <si>
+    <t>Lesson Key Take-Aways</t>
+  </si>
+  <si>
+    <t>Reward System Brainstorm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan 25th       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan 27th       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan 28th      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     </t>
+  </si>
+  <si>
+    <t>JSON Read/Write</t>
+  </si>
+  <si>
+    <t>Feb4</t>
+  </si>
+  <si>
+    <t>Understand requirements for flow charts for Nocti</t>
+  </si>
+  <si>
+    <t>Solve a variety of Javascript problems that may appear on the Nocti</t>
+  </si>
+  <si>
+    <t>Prepare DocPac Data for Analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single: Nocti Flowchart Perparation </t>
+  </si>
+  <si>
+    <t>Teams: DocPac Digitalization</t>
+  </si>
+  <si>
+    <t>Pairs: JS Challenge Pt. 7</t>
+  </si>
+  <si>
+    <t>Pairs: JS Challenge Pt. 8</t>
+  </si>
+  <si>
+    <t>Single: Nocti Flowchart Preparation</t>
+  </si>
+  <si>
+    <t>New Grading System</t>
+  </si>
+  <si>
+    <t>Single: This assignment should only be completed by you. Do not share</t>
+  </si>
+  <si>
+    <t>Pairs: Only one or two people may complete this assignment. Do not share</t>
+  </si>
+  <si>
+    <t>Teams: Your whole team can complete and share this project with each other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jan 31st       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feb 4th          </t>
   </si>
 </sst>
 </file>
@@ -800,8 +1013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC9A7DB5-AC61-4B29-BFC8-F37F5680E13D}">
   <dimension ref="A1:B136"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1028,6 +1241,126 @@
         <v>129</v>
       </c>
     </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B36" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B37" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B38" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B40" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B41" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B42" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B43" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B45" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B46" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B48" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B49" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B50" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B52" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B53" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B54" t="s">
+        <v>198</v>
+      </c>
+    </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
     </row>
@@ -1046,10 +1379,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D30F3F7-430A-4866-93CA-CC57104C99B6}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1184,6 +1517,248 @@
         <v>131</v>
       </c>
     </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B32" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B35" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B38" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B41" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B44" t="s">
+        <v>84</v>
+      </c>
+      <c r="C44" t="s">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1191,10 +1766,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D695B668-03FA-4899-A177-F8CD6E2821D4}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H62" sqref="H62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1477,6 +2052,237 @@
         <v>131</v>
       </c>
     </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B33" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B35" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B36" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B39" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B40" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B41" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B45" t="s">
+        <v>85</v>
+      </c>
+      <c r="C45" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B47" t="s">
+        <v>84</v>
+      </c>
+      <c r="C47" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B49" t="s">
+        <v>14</v>
+      </c>
+      <c r="C49" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B50" t="s">
+        <v>14</v>
+      </c>
+      <c r="C50" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B51" t="s">
+        <v>84</v>
+      </c>
+      <c r="C51" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B53" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B54" t="s">
+        <v>67</v>
+      </c>
+      <c r="C54" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B55" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B56" t="s">
+        <v>14</v>
+      </c>
+      <c r="C56" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B57" t="s">
+        <v>84</v>
+      </c>
+      <c r="C57" t="s">
+        <v>86</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1484,10 +2290,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81AAD0C2-9933-4E01-8339-7824E22AD9C7}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1572,6 +2378,70 @@
         <v>92</v>
       </c>
     </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B18" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B22" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B26" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B27" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B28" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B29" t="s">
+        <v>207</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1579,10 +2449,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4E6F3D7-8229-400D-93B9-D8522A9EF6FE}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2116,6 +2986,335 @@
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
         <v>120</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D43" t="s">
+        <v>33</v>
+      </c>
+      <c r="E43" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D44" t="s">
+        <v>33</v>
+      </c>
+      <c r="E44" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D45" t="s">
+        <v>58</v>
+      </c>
+      <c r="E45" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D46" t="s">
+        <v>58</v>
+      </c>
+      <c r="E46" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D47" t="s">
+        <v>58</v>
+      </c>
+      <c r="E47" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D49" t="s">
+        <v>33</v>
+      </c>
+      <c r="E49" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D50" t="s">
+        <v>58</v>
+      </c>
+      <c r="E50" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D51" t="s">
+        <v>33</v>
+      </c>
+      <c r="E51" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D52" t="s">
+        <v>58</v>
+      </c>
+      <c r="E52" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D53" t="s">
+        <v>58</v>
+      </c>
+      <c r="E53" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D54" t="s">
+        <v>33</v>
+      </c>
+      <c r="E54" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D55" t="s">
+        <v>33</v>
+      </c>
+      <c r="E55" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D57" t="s">
+        <v>33</v>
+      </c>
+      <c r="E57" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D58" t="s">
+        <v>58</v>
+      </c>
+      <c r="E58" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D59" t="s">
+        <v>33</v>
+      </c>
+      <c r="E59" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D60" t="s">
+        <v>33</v>
+      </c>
+      <c r="E60" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B61" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D62" t="s">
+        <v>33</v>
+      </c>
+      <c r="E62" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D63" t="s">
+        <v>58</v>
+      </c>
+      <c r="E63" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D64" t="s">
+        <v>33</v>
+      </c>
+      <c r="E64" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D65" t="s">
+        <v>33</v>
+      </c>
+      <c r="E65" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B66" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D67" t="s">
+        <v>33</v>
+      </c>
+      <c r="E67" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D68" t="s">
+        <v>33</v>
+      </c>
+      <c r="E68" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2130,15 +3329,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100651E00D2AC2DD14EB60A774F4411C2DE" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5fa4770c7f3533901a642ebc136dfacc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a226a929-813b-4430-a398-5fab01598312" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5ce44c3146c3c9503a47426e7c52d1ce" ns3:_="">
     <xsd:import namespace="a226a929-813b-4430-a398-5fab01598312"/>
@@ -2322,31 +3512,32 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C285CC4-3253-4C12-975B-4002A1BA8DE9}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="a226a929-813b-4430-a398-5fab01598312"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a226a929-813b-4430-a398-5fab01598312"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73DF8B37-3924-4B7F-92F7-3C408EBADD86}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44355066-F617-4086-8F16-3629E3FE7CA3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2362,4 +3553,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73DF8B37-3924-4B7F-92F7-3C408EBADD86}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>